<commit_message>
Atuallização do update nos endpoints
</commit_message>
<xml_diff>
--- a/Documentação/Mapeamento REST/Mapeamento.xlsx
+++ b/Documentação/Mapeamento REST/Mapeamento.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STS4\Fatec\tg-1\tg-1\Documentação\Mapeamento REST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cursos\FATEC\5 - Semestre\TG I\Projetos\tg\Documentação\Mapeamento REST\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CADBBF1-FA64-4C17-B082-757A1E2C2B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-105" windowWidth="30000" windowHeight="13170"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="30000" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="81">
   <si>
     <t>Verbo HTTP</t>
   </si>
@@ -215,9 +216,6 @@
     <t>admin, sistema</t>
   </si>
   <si>
-    <t>Pesquisar</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -255,12 +253,27 @@
   </si>
   <si>
     <t>Endpoint (/usuarios)</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Testes</t>
+  </si>
+  <si>
+    <t>OK - Verificar se existe o ID</t>
+  </si>
+  <si>
+    <t>Não retorna a lista</t>
+  </si>
+  <si>
+    <t>Corrigir para o CPF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -311,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -519,11 +532,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -549,6 +612,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,13 +640,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>331470</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
@@ -586,7 +656,7 @@
         <xdr:cNvPr id="2" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D796DA6B-9DBC-BD88-4DF5-614709BED0EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D796DA6B-9DBC-BD88-4DF5-614709BED0EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -631,13 +701,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>464820</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
@@ -647,7 +717,7 @@
         <xdr:cNvPr id="3" name="Imagem 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CA64FE14-AB7B-2EFE-19C2-041B35407560}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA64FE14-AB7B-2EFE-19C2-041B35407560}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -955,44 +1025,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="H2" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="18"/>
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1006,17 +1078,20 @@
       <c r="E3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
@@ -1030,28 +1105,30 @@
       <c r="E4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="19"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
@@ -1065,11 +1142,12 @@
       <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="20"/>
+      <c r="G7" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1083,20 +1161,22 @@
       <c r="E8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="22"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="19"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
@@ -1110,11 +1190,12 @@
       <c r="E11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="20"/>
+      <c r="G11" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1128,9 +1209,14 @@
       <c r="E12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1144,9 +1230,12 @@
       <c r="E13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1160,11 +1249,14 @@
       <c r="E14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1178,20 +1270,26 @@
       <c r="E15" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="19"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -1205,11 +1303,12 @@
       <c r="E18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="20"/>
+      <c r="G18" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
@@ -1223,11 +1322,12 @@
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="23"/>
+      <c r="G19" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1241,9 +1341,10 @@
       <c r="E20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="23"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -1255,20 +1356,22 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="22"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="19"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>0</v>
       </c>
@@ -1282,11 +1385,14 @@
       <c r="E24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
@@ -1300,11 +1406,14 @@
       <c r="E25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -1318,11 +1427,14 @@
       <c r="E26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1336,11 +1448,14 @@
       <c r="E27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -1354,22 +1469,26 @@
       <c r="E28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="19"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>0</v>
       </c>
@@ -1383,11 +1502,14 @@
       <c r="E31" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>4</v>
       </c>
@@ -1401,11 +1523,14 @@
       <c r="E32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
@@ -1419,11 +1544,14 @@
       <c r="E33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1437,11 +1565,14 @@
       <c r="E34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
@@ -1455,22 +1586,26 @@
       <c r="E35" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="19"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>0</v>
       </c>
@@ -1484,11 +1619,12 @@
       <c r="E38" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="20"/>
+      <c r="G38" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
@@ -1502,11 +1638,14 @@
       <c r="E39" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -1520,11 +1659,14 @@
       <c r="E40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
@@ -1538,11 +1680,14 @@
       <c r="E41" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -1556,22 +1701,26 @@
       <c r="E42" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
-      <c r="F44" s="18"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="19"/>
+      <c r="G44" s="18"/>
+    </row>
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>0</v>
       </c>
@@ -1585,11 +1734,12 @@
       <c r="E45" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="20"/>
+      <c r="G45" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>4</v>
       </c>
@@ -1603,11 +1753,14 @@
       <c r="E46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -1621,11 +1774,14 @@
       <c r="E47" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>6</v>
       </c>
@@ -1639,11 +1795,14 @@
       <c r="E48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F48" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -1657,22 +1816,26 @@
       <c r="E49" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F49" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
-      <c r="F51" s="18"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="19"/>
+      <c r="G51" s="18"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>0</v>
       </c>
@@ -1686,11 +1849,12 @@
       <c r="E52" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="20"/>
+      <c r="G52" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>4</v>
       </c>
@@ -1704,11 +1868,12 @@
       <c r="E53" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="23"/>
+      <c r="G53" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
@@ -1722,11 +1887,12 @@
       <c r="E54" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="23"/>
+      <c r="G54" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>6</v>
       </c>
@@ -1740,11 +1906,12 @@
       <c r="E55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="23"/>
+      <c r="G55" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
@@ -1758,22 +1925,24 @@
       <c r="E56" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F56" s="22"/>
+      <c r="G56" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
-      <c r="F58" s="18"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="19"/>
+      <c r="G58" s="18"/>
+    </row>
+    <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>0</v>
       </c>
@@ -1787,11 +1956,12 @@
       <c r="E59" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="20"/>
+      <c r="G59" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>4</v>
       </c>
@@ -1805,11 +1975,12 @@
       <c r="E60" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="23"/>
+      <c r="G60" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -1823,11 +1994,12 @@
       <c r="E61" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="23"/>
+      <c r="G61" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>6</v>
       </c>
@@ -1841,11 +2013,12 @@
       <c r="E62" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F62" s="23"/>
+      <c r="G62" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>7</v>
       </c>
@@ -1859,22 +2032,24 @@
       <c r="E63" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F63" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F63" s="22"/>
+      <c r="G63" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
       <c r="E65" s="17"/>
-      <c r="F65" s="18"/>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F65" s="19"/>
+      <c r="G65" s="18"/>
+    </row>
+    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>0</v>
       </c>
@@ -1888,11 +2063,12 @@
       <c r="E66" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="F66" s="20"/>
+      <c r="G66" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>4</v>
       </c>
@@ -1906,11 +2082,12 @@
       <c r="E67" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="23"/>
+      <c r="G67" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>5</v>
       </c>
@@ -1924,11 +2101,12 @@
       <c r="E68" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="23"/>
+      <c r="G68" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>6</v>
       </c>
@@ -1942,11 +2120,12 @@
       <c r="E69" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F69" s="23"/>
+      <c r="G69" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
@@ -1960,23 +2139,24 @@
       <c r="E70" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F70" s="6" t="s">
-        <v>64</v>
+      <c r="F70" s="22"/>
+      <c r="G70" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A44:G44"/>
+    <mergeCell ref="A51:G51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>